<commit_message>
Lack of Introduction and Excutive summary
</commit_message>
<xml_diff>
--- a/CalculationTables.xlsx
+++ b/CalculationTables.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="144">
   <si>
     <t>Yearly Range</t>
   </si>
@@ -455,6 +455,42 @@
   </si>
   <si>
     <t>Hand Calculation</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <t>Wall</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Appliances</t>
+  </si>
+  <si>
+    <t>Radiation</t>
+  </si>
+  <si>
+    <t>CAMEL</t>
+  </si>
+  <si>
+    <t>Heating load</t>
+  </si>
+  <si>
+    <t>camel</t>
+  </si>
+  <si>
+    <t>sensible</t>
+  </si>
+  <si>
+    <t>latent</t>
+  </si>
+  <si>
+    <t>hand calculation</t>
   </si>
 </sst>
 </file>
@@ -636,7 +672,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -707,13 +743,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -728,16 +779,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1143,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R139"/>
+  <dimension ref="A1:R167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="F138" sqref="F138"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164:E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1244,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1232,10 +1277,10 @@
       <c r="K2" s="4">
         <v>0</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="28"/>
+      <c r="N2" s="33"/>
       <c r="O2" s="5" t="s">
         <v>36</v>
       </c>
@@ -1244,7 +1289,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1275,10 +1320,10 @@
       <c r="K3" s="4">
         <v>0</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="23"/>
+      <c r="N3" s="28"/>
       <c r="O3" s="4">
         <v>0.72499999999999998</v>
       </c>
@@ -1298,7 +1343,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="28" t="s">
         <v>26</v>
       </c>
       <c r="N4" s="4" t="s">
@@ -1312,7 +1357,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M5" s="23"/>
+      <c r="M5" s="28"/>
       <c r="N5" s="4" t="s">
         <v>51</v>
       </c>
@@ -1324,20 +1369,20 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="M6" s="23" t="s">
+      <c r="D6" s="29"/>
+      <c r="M6" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="23"/>
+      <c r="N6" s="28"/>
       <c r="O6" s="4" t="s">
         <v>29</v>
       </c>
@@ -1346,16 +1391,16 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
       <c r="O7" s="4" t="s">
         <v>30</v>
       </c>
@@ -1376,10 +1421,10 @@
       <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="23" t="s">
+      <c r="M8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="23"/>
+      <c r="N8" s="28"/>
       <c r="O8" s="4">
         <v>0.56200000000000006</v>
       </c>
@@ -1402,10 +1447,10 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="M11" s="29" t="s">
+      <c r="M11" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="30"/>
+      <c r="N11" s="35"/>
       <c r="O11" s="10" t="s">
         <v>56</v>
       </c>
@@ -1429,10 +1474,10 @@
       <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="N12" s="23"/>
+      <c r="N12" s="28"/>
       <c r="O12" s="4">
         <v>0.72499999999999998</v>
       </c>
@@ -1457,7 +1502,7 @@
       <c r="C13" s="4">
         <v>1.38</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="M13" s="28" t="s">
         <v>26</v>
       </c>
       <c r="N13" s="4" t="s">
@@ -1483,7 +1528,7 @@
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="M14" s="23"/>
+      <c r="M14" s="28"/>
       <c r="N14" s="4" t="s">
         <v>51</v>
       </c>
@@ -1502,7 +1547,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="30" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1511,10 +1556,10 @@
       <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="23"/>
+      <c r="N15" s="28"/>
       <c r="O15" s="4" t="s">
         <v>29</v>
       </c>
@@ -1530,15 +1575,15 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
       <c r="O16" s="4" t="s">
         <v>30</v>
       </c>
@@ -1563,10 +1608,10 @@
       <c r="C17" s="4">
         <v>1.78</v>
       </c>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="N17" s="23"/>
+      <c r="N17" s="28"/>
       <c r="O17" s="4">
         <v>0.56200000000000006</v>
       </c>
@@ -1802,13 +1847,13 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
       <c r="F35" s="4">
         <f>SUM(F30:F34)</f>
         <v>6483.7139999999999</v>
@@ -1882,13 +1927,13 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
       <c r="F40" s="4">
         <f>SUM(F38:F39)</f>
         <v>198616</v>
@@ -1958,13 +2003,13 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
       <c r="F45" s="4">
         <f>SUM(F43:F44)</f>
         <v>42602.8</v>
@@ -2036,13 +2081,13 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
       <c r="F50" s="4">
         <f>SUM(F48:F49)</f>
         <v>128392</v>
@@ -2200,13 +2245,13 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
+      <c r="A59" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
       <c r="F59" s="4">
         <f>SUM(F55:F58)</f>
         <v>19188.674999999999</v>
@@ -2360,13 +2405,13 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
       <c r="F66" s="4">
         <f>SUM(F62:F65)</f>
         <v>88267.904999999999</v>
@@ -2477,11 +2522,11 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="25" t="s">
+      <c r="A76" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="27"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
@@ -2517,11 +2562,11 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="26" t="s">
+      <c r="A81" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B81" s="26"/>
-      <c r="C81" s="26"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
@@ -2543,12 +2588,12 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="22" t="s">
+      <c r="A88" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B88" s="22"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="22"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
@@ -2719,29 +2764,29 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="25" t="s">
+      <c r="A102" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B102" s="25"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="22" t="s">
+      <c r="A103" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B103" s="22" t="s">
+      <c r="B103" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C103" s="22"/>
-      <c r="D103" s="22" t="s">
+      <c r="C103" s="26"/>
+      <c r="D103" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="E103" s="22"/>
+      <c r="E103" s="26"/>
     </row>
     <row r="104" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="22"/>
+      <c r="A104" s="26"/>
       <c r="B104" s="21" t="s">
         <v>111</v>
       </c>
@@ -2814,13 +2859,13 @@
         <v>4728</v>
       </c>
       <c r="C108" s="20">
-        <v>3993</v>
+        <v>3328</v>
       </c>
       <c r="D108" s="20">
         <v>11970</v>
       </c>
       <c r="E108" s="20">
-        <v>9266</v>
+        <v>7721</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2833,7 +2878,7 @@
       </c>
       <c r="C109" s="20">
         <f t="shared" ref="C109:E109" si="7">SUM(C105:C108)</f>
-        <v>6903</v>
+        <v>6238</v>
       </c>
       <c r="D109" s="20">
         <f t="shared" si="7"/>
@@ -2841,33 +2886,33 @@
       </c>
       <c r="E109" s="20">
         <f t="shared" si="7"/>
-        <v>18254</v>
+        <v>16709</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="25" t="s">
+      <c r="A111" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="B111" s="25"/>
-      <c r="C111" s="25"/>
-      <c r="D111" s="25"/>
-      <c r="E111" s="25"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="27"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="22" t="s">
+      <c r="A112" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B112" s="22" t="s">
+      <c r="B112" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C112" s="22"/>
-      <c r="D112" s="22" t="s">
+      <c r="C112" s="26"/>
+      <c r="D112" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="E112" s="22"/>
+      <c r="E112" s="26"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="22"/>
+      <c r="A113" s="26"/>
       <c r="B113" s="21" t="s">
         <v>111</v>
       </c>
@@ -2971,29 +3016,29 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="22" t="s">
+      <c r="A121" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B121" s="22"/>
-      <c r="C121" s="22"/>
-      <c r="D121" s="22"/>
-      <c r="E121" s="22"/>
+      <c r="B121" s="26"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="26"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="22" t="s">
+      <c r="A122" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B122" s="22" t="s">
+      <c r="B122" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C122" s="22"/>
-      <c r="D122" s="22" t="s">
+      <c r="C122" s="26"/>
+      <c r="D122" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="E122" s="22"/>
+      <c r="E122" s="26"/>
     </row>
     <row r="123" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="22"/>
+      <c r="A123" s="26"/>
       <c r="B123" s="21" t="s">
         <v>118</v>
       </c>
@@ -3032,13 +3077,15 @@
         <v>15313</v>
       </c>
       <c r="C125" s="20">
-        <v>6903</v>
+        <f>C109</f>
+        <v>6238</v>
       </c>
       <c r="D125" s="20">
         <v>42576</v>
       </c>
       <c r="E125" s="20">
-        <v>18254</v>
+        <f>E109</f>
+        <v>16709</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,7 +3098,7 @@
       </c>
       <c r="C126" s="20">
         <f t="shared" ref="C126:E126" si="9">C124+C125</f>
-        <v>6903</v>
+        <v>6238</v>
       </c>
       <c r="D126" s="20">
         <f t="shared" si="9"/>
@@ -3059,33 +3106,33 @@
       </c>
       <c r="E126" s="20">
         <f t="shared" si="9"/>
-        <v>18254</v>
+        <v>16709</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="22" t="s">
+      <c r="A127" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B127" s="22"/>
-      <c r="C127" s="22"/>
-      <c r="D127" s="22"/>
-      <c r="E127" s="22"/>
+      <c r="B127" s="26"/>
+      <c r="C127" s="26"/>
+      <c r="D127" s="26"/>
+      <c r="E127" s="26"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="22" t="s">
+      <c r="A128" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B128" s="22" t="s">
+      <c r="B128" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C128" s="22"/>
-      <c r="D128" s="22" t="s">
+      <c r="C128" s="26"/>
+      <c r="D128" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="E128" s="22"/>
+      <c r="E128" s="26"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="22"/>
+      <c r="A129" s="26"/>
       <c r="B129" s="21" t="s">
         <v>118</v>
       </c>
@@ -3155,6 +3202,10 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B135" s="26"/>
       <c r="C135" s="26" t="s">
         <v>130</v>
       </c>
@@ -3165,97 +3216,523 @@
       <c r="F135" s="26"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C136" s="34" t="s">
+      <c r="A136" s="26"/>
+      <c r="B136" s="26"/>
+      <c r="C136" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D136" s="34" t="s">
+      <c r="D136" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="E136" s="34" t="s">
+      <c r="E136" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="F136" s="34" t="s">
+      <c r="F136" s="22" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="26" t="s">
+      <c r="A137" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B137" s="11" t="s">
+      <c r="B137" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C137" s="11">
+      <c r="C137" s="23">
         <v>16602</v>
       </c>
-      <c r="D137" s="11">
+      <c r="D137" s="23">
         <v>53414</v>
       </c>
-      <c r="E137" s="11">
+      <c r="E137" s="23">
         <v>16222</v>
       </c>
-      <c r="F137" s="11">
+      <c r="F137" s="23">
         <v>48545</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="26"/>
-      <c r="B138" s="11" t="s">
+      <c r="A138" s="28"/>
+      <c r="B138" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="C138" s="11">
+      <c r="C138" s="23">
         <v>6741</v>
       </c>
-      <c r="D138" s="11">
+      <c r="D138" s="23">
         <v>17950</v>
       </c>
-      <c r="E138" s="11">
+      <c r="E138" s="23">
         <v>6903</v>
       </c>
-      <c r="F138" s="11">
+      <c r="F138" s="23">
         <v>18254</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="11" t="s">
+      <c r="A139" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B139" s="11" t="s">
+      <c r="B139" s="23" t="s">
         <v>118</v>
       </c>
+      <c r="C139" s="23">
+        <v>10896</v>
+      </c>
+      <c r="D139" s="23">
+        <v>31850</v>
+      </c>
+      <c r="E139" s="23">
+        <v>9634</v>
+      </c>
+      <c r="F139" s="23">
+        <v>12017</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B141" s="26"/>
+      <c r="C141" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D141" s="26"/>
+      <c r="E141" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F141" s="26"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="26"/>
+      <c r="B142" s="26"/>
+      <c r="C142" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D142" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E142" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F142" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B143" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C143" s="23">
+        <v>94</v>
+      </c>
+      <c r="D143" s="23">
+        <v>0</v>
+      </c>
+      <c r="E143" s="23">
+        <v>140</v>
+      </c>
+      <c r="F143" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="28"/>
+      <c r="B144" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C144" s="23">
+        <v>572</v>
+      </c>
+      <c r="D144" s="23">
+        <v>0</v>
+      </c>
+      <c r="E144" s="23">
+        <v>248</v>
+      </c>
+      <c r="F144" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="28"/>
+      <c r="B145" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C145" s="23">
+        <v>521</v>
+      </c>
+      <c r="D145" s="23">
+        <v>0</v>
+      </c>
+      <c r="E145" s="23">
+        <v>521</v>
+      </c>
+      <c r="F145" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B146" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C146" s="23">
+        <v>3600</v>
+      </c>
+      <c r="D146" s="23">
+        <v>2900</v>
+      </c>
+      <c r="E146" s="23">
+        <v>3240</v>
+      </c>
+      <c r="F146" s="23">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="28"/>
+      <c r="B147" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C147" s="23">
+        <v>2500</v>
+      </c>
+      <c r="D147" s="23">
+        <v>300</v>
+      </c>
+      <c r="E147" s="23">
+        <v>2542</v>
+      </c>
+      <c r="F147" s="23">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="28"/>
+      <c r="B148" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C148" s="23">
+        <v>4408</v>
+      </c>
+      <c r="D148" s="23">
+        <v>0</v>
+      </c>
+      <c r="E148" s="23">
+        <v>4803</v>
+      </c>
+      <c r="F148" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="28"/>
+      <c r="B149" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C149" s="23">
+        <v>4776</v>
+      </c>
+      <c r="D149" s="23">
+        <v>3541</v>
+      </c>
+      <c r="E149" s="23">
+        <v>4728</v>
+      </c>
+      <c r="F149" s="23">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B150" s="37"/>
+      <c r="C150" s="23">
+        <f>SUM(C143:C149)</f>
+        <v>16471</v>
+      </c>
+      <c r="D150" s="23">
+        <f>SUM(D143:D149)</f>
+        <v>6741</v>
+      </c>
+      <c r="E150" s="23">
+        <f>SUM(E143:E149)</f>
+        <v>16222</v>
+      </c>
+      <c r="F150" s="23">
+        <f>SUM(F143:F149)</f>
+        <v>6238</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B152" s="26"/>
+      <c r="C152" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D152" s="26"/>
+      <c r="E152" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F152" s="26"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="26"/>
+      <c r="B153" s="26"/>
+      <c r="C153" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D153" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E153" s="22"/>
+      <c r="F153" s="22"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B154" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C154" s="23">
+        <v>626</v>
+      </c>
+      <c r="D154" s="23">
+        <v>0</v>
+      </c>
+      <c r="E154" s="23">
+        <v>739</v>
+      </c>
+      <c r="F154" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="28"/>
+      <c r="B155" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C155" s="23">
+        <v>8135</v>
+      </c>
+      <c r="D155" s="23">
+        <v>0</v>
+      </c>
+      <c r="E155" s="23">
+        <v>1219</v>
+      </c>
+      <c r="F155" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="28"/>
+      <c r="B156" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C156" s="23">
+        <v>3995</v>
+      </c>
+      <c r="D156" s="23">
+        <v>0</v>
+      </c>
+      <c r="E156" s="23">
+        <v>3994</v>
+      </c>
+      <c r="F156" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B157" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C157" s="23">
+        <v>10080</v>
+      </c>
+      <c r="D157" s="23">
+        <v>8120</v>
+      </c>
+      <c r="E157" s="23">
+        <v>9072</v>
+      </c>
+      <c r="F157" s="23">
+        <v>7308</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="28"/>
+      <c r="B158" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C158" s="23">
+        <v>9400</v>
+      </c>
+      <c r="D158" s="23">
+        <v>1700</v>
+      </c>
+      <c r="E158" s="23">
+        <v>9390</v>
+      </c>
+      <c r="F158" s="23">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="28"/>
+      <c r="B159" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C159" s="23">
+        <v>10602</v>
+      </c>
+      <c r="D159" s="23">
+        <v>0</v>
+      </c>
+      <c r="E159" s="23">
+        <v>12144</v>
+      </c>
+      <c r="F159" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="28"/>
+      <c r="B160" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C160" s="23">
+        <v>10967</v>
+      </c>
+      <c r="D160" s="23">
+        <v>8130</v>
+      </c>
+      <c r="E160" s="23">
+        <v>11970</v>
+      </c>
+      <c r="F160" s="23">
+        <v>7721</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B161" s="37"/>
+      <c r="C161" s="23">
+        <f>SUM(C154:C160)</f>
+        <v>53805</v>
+      </c>
+      <c r="D161" s="23">
+        <f>SUM(D154:D160)</f>
+        <v>17950</v>
+      </c>
+      <c r="E161" s="23">
+        <f t="shared" ref="E161:F161" si="11">SUM(E154:E160)</f>
+        <v>48528</v>
+      </c>
+      <c r="F161" s="23">
+        <f t="shared" si="11"/>
+        <v>16709</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B164" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C164" s="26"/>
+      <c r="D164" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E164" s="26"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="26"/>
+      <c r="B165" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C165" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D165" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E165" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B166" s="23">
+        <v>10896</v>
+      </c>
+      <c r="C166" s="23">
+        <v>31850</v>
+      </c>
+      <c r="D166" s="23">
+        <v>9670</v>
+      </c>
+      <c r="E166" s="23">
+        <v>29019</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B167" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C167" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D167" s="23">
+        <v>9383</v>
+      </c>
+      <c r="E167" s="23">
+        <v>23164</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="E135:F135"/>
-    <mergeCell ref="A127:E127"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="A121:E121"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="A102:E102"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M6:N7"/>
-    <mergeCell ref="M8:N8"/>
+  <mergeCells count="59">
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="A152:B153"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="E152:F152"/>
+    <mergeCell ref="A154:A156"/>
+    <mergeCell ref="A157:A160"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="E141:F141"/>
+    <mergeCell ref="A141:B142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A149"/>
     <mergeCell ref="A88:D88"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="M13:M14"/>
@@ -3269,6 +3746,37 @@
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="A59:E59"/>
     <mergeCell ref="A66:E66"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M6:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="A121:E121"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="E135:F135"/>
+    <mergeCell ref="A127:E127"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="A135:B136"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>